<commit_message>
Correction in the Order of Alternaria
</commit_message>
<xml_diff>
--- a/Data/TABLE_S2_COM2.xlsx
+++ b/Data/TABLE_S2_COM2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valeriehofstetter/Desktop/SOUR ROT SUBMISSION/FINAL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U80821784\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D461A1E5-ACC2-8E46-A8D5-5D6F2DCFA5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B6CC89-30AE-4788-977C-64E366A60313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="760" windowWidth="25040" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="2" r:id="rId1"/>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="479">
   <si>
     <t>Cephalotrichum gorgonifer</t>
   </si>
@@ -177,9 +175,6 @@
   </si>
   <si>
     <t>Order; family (after GenBank)</t>
-  </si>
-  <si>
-    <t>Pleosporineae; Pleosporaceae</t>
   </si>
   <si>
     <t>Xylariales; Apiosporaceae</t>
@@ -4314,28 +4309,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2328C5AA-A247-BD4D-9F3D-557A978B55F4}">
   <dimension ref="A1:U93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36" style="2" customWidth="1"/>
-    <col min="2" max="14" width="4.83203125" style="20" customWidth="1"/>
+    <col min="2" max="14" width="4.796875" style="20" customWidth="1"/>
     <col min="15" max="15" width="44" style="15" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" style="13"/>
+    <col min="16" max="16" width="10.796875" style="13"/>
     <col min="17" max="17" width="13" style="28" customWidth="1"/>
-    <col min="18" max="18" width="33.6640625" style="15" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" style="13" customWidth="1"/>
-    <col min="20" max="20" width="11.1640625" style="13" customWidth="1"/>
+    <col min="18" max="18" width="33.69921875" style="15" customWidth="1"/>
+    <col min="19" max="19" width="12.296875" style="13" customWidth="1"/>
+    <col min="20" max="20" width="11.19921875" style="13" customWidth="1"/>
     <col min="21" max="21" width="34" style="15" customWidth="1"/>
     <col min="22" max="22" width="27" style="2" customWidth="1"/>
-    <col min="23" max="16384" width="10.83203125" style="2"/>
+    <col min="23" max="16384" width="10.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="119" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" ht="118.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -4358,63 +4353,63 @@
       <c r="T1" s="31"/>
       <c r="U1" s="32"/>
     </row>
-    <row r="2" spans="1:21" ht="102" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>366</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="D2" s="17" t="s">
         <v>367</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="17" t="s">
         <v>368</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="17" t="s">
         <v>369</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>370</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="H2" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>371</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>379</v>
-      </c>
-      <c r="I2" s="17" t="s">
+      <c r="J2" s="17" t="s">
         <v>372</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="K2" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="L2" s="18" t="s">
         <v>374</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="M2" s="17" t="s">
         <v>375</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="N2" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="N2" s="17" t="s">
-        <v>377</v>
-      </c>
       <c r="O2" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="R2" s="18" t="s">
         <v>362</v>
       </c>
-      <c r="P2" s="17" t="s">
-        <v>341</v>
-      </c>
-      <c r="Q2" s="26" t="s">
-        <v>342</v>
-      </c>
-      <c r="R2" s="18" t="s">
-        <v>363</v>
-      </c>
       <c r="S2" s="19" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="T2" s="19" t="s">
         <v>28</v>
@@ -4423,7 +4418,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -4439,7 +4434,7 @@
         <v>26</v>
       </c>
       <c r="Q3" s="29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="R3" s="11" t="s">
         <v>27</v>
@@ -4451,12 +4446,12 @@
         <v>100</v>
       </c>
       <c r="U3" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" s="21">
         <v>3</v>
@@ -4471,7 +4466,7 @@
         <v>30</v>
       </c>
       <c r="Q4" s="29" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R4" s="11" t="s">
         <v>31</v>
@@ -4483,12 +4478,12 @@
         <v>100</v>
       </c>
       <c r="U4" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D5" s="21">
         <v>3</v>
@@ -4503,7 +4498,7 @@
         <v>32</v>
       </c>
       <c r="Q5" s="29" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="R5" s="11" t="s">
         <v>31</v>
@@ -4515,10 +4510,10 @@
         <v>100</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -4544,7 +4539,7 @@
         <v>34</v>
       </c>
       <c r="Q6" s="29" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="R6" s="11" t="s">
         <v>35</v>
@@ -4556,12 +4551,12 @@
         <v>100</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N7" s="21">
         <v>1</v>
@@ -4573,24 +4568,24 @@
         <v>36</v>
       </c>
       <c r="Q7" s="29" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="R7" s="11" t="s">
         <v>35</v>
       </c>
       <c r="S7" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="T7" s="14">
         <v>90</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L8" s="21">
         <v>2</v>
@@ -4602,24 +4597,24 @@
         <v>37</v>
       </c>
       <c r="Q8" s="29" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="R8" s="11" t="s">
         <v>35</v>
       </c>
       <c r="S8" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="T8" s="14">
         <v>100</v>
       </c>
       <c r="U8" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B9" s="21">
         <v>1</v>
@@ -4634,24 +4629,24 @@
         <v>38</v>
       </c>
       <c r="Q9" s="29" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="R9" s="11" t="s">
         <v>39</v>
       </c>
       <c r="S9" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="T9" s="14">
         <v>100</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C10" s="21">
         <v>2</v>
@@ -4663,22 +4658,22 @@
         <v>41</v>
       </c>
       <c r="Q10" s="29" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="R10" s="11" t="s">
         <v>42</v>
       </c>
       <c r="S10" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="T10" s="14">
         <v>100</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -4686,17 +4681,17 @@
         <v>1</v>
       </c>
       <c r="O11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="P11" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="P11" s="12" t="s">
+      <c r="Q11" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="R11" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="Q11" s="29" t="s">
-        <v>403</v>
-      </c>
-      <c r="R11" s="11" t="s">
-        <v>51</v>
-      </c>
       <c r="S11" s="13">
         <v>100</v>
       </c>
@@ -4704,12 +4699,12 @@
         <v>100</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="34" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C12" s="21">
         <v>10</v>
@@ -4733,13 +4728,13 @@
         <v>43</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q12" s="29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S12" s="13">
         <v>100</v>
@@ -4748,12 +4743,12 @@
         <v>100</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="31.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F13" s="23">
         <v>4</v>
@@ -4765,24 +4760,24 @@
         <v>44</v>
       </c>
       <c r="Q13" s="29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S13" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="T13" s="14">
         <v>100</v>
       </c>
       <c r="U13" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D14" s="21">
         <v>3</v>
@@ -4791,27 +4786,27 @@
         <v>43</v>
       </c>
       <c r="P14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q14" s="29" t="s">
+        <v>405</v>
+      </c>
+      <c r="R14" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="Q14" s="29" t="s">
-        <v>406</v>
-      </c>
-      <c r="R14" s="11" t="s">
-        <v>54</v>
-      </c>
       <c r="S14" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="T14" s="14">
         <v>100</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D15" s="21">
         <v>6</v>
@@ -4826,13 +4821,13 @@
         <v>43</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q15" s="29" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="S15" s="14">
         <v>100</v>
@@ -4841,12 +4836,12 @@
         <v>100</v>
       </c>
       <c r="U15" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C16" s="21">
         <v>2</v>
@@ -4855,14 +4850,14 @@
         <v>43</v>
       </c>
       <c r="P16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q16" s="28" t="s">
+        <v>407</v>
+      </c>
+      <c r="R16" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="Q16" s="28" t="s">
-        <v>408</v>
-      </c>
-      <c r="R16" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="S16" s="13">
         <v>100</v>
       </c>
@@ -4870,10 +4865,10 @@
         <v>100</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
@@ -4884,13 +4879,13 @@
         <v>43</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q17" s="29" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="S17" s="13">
         <v>100</v>
@@ -4899,10 +4894,10 @@
         <v>100</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -4910,16 +4905,16 @@
         <v>3</v>
       </c>
       <c r="O18" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="P18" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q18" s="27" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S18" s="16">
         <v>100</v>
@@ -4928,27 +4923,27 @@
         <v>100</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="34" x14ac:dyDescent="0.15">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F19" s="24">
         <v>4</v>
       </c>
       <c r="O19" s="15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q19" s="27" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="R19" s="15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="S19" s="16">
         <v>100</v>
@@ -4957,41 +4952,41 @@
         <v>100</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G20" s="24">
         <v>3</v>
       </c>
       <c r="O20" s="15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P20" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q20" s="27" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="R20" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="S20" s="16">
+        <v>100</v>
+      </c>
+      <c r="T20" s="13">
+        <v>100</v>
+      </c>
+      <c r="U20" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="S20" s="16">
-        <v>100</v>
-      </c>
-      <c r="T20" s="13">
-        <v>100</v>
-      </c>
-      <c r="U20" s="10" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B21" s="24">
         <v>2</v>
@@ -5000,16 +4995,16 @@
         <v>2</v>
       </c>
       <c r="O21" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P21" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Q21" s="27" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="R21" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="S21" s="13">
         <v>100</v>
@@ -5018,10 +5013,10 @@
         <v>100</v>
       </c>
       <c r="U21" s="10" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
@@ -5032,17 +5027,17 @@
         <v>2</v>
       </c>
       <c r="O22" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="P22" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="P22" s="12" t="s">
+      <c r="Q22" s="27" t="s">
+        <v>409</v>
+      </c>
+      <c r="R22" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="Q22" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="R22" s="11" t="s">
-        <v>62</v>
-      </c>
       <c r="S22" s="13">
         <v>100</v>
       </c>
@@ -5050,10 +5045,10 @@
         <v>100</v>
       </c>
       <c r="U22" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" s="7" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" s="7" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>23</v>
       </c>
@@ -5073,28 +5068,28 @@
       <c r="M23" s="25"/>
       <c r="N23" s="25"/>
       <c r="O23" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="P23" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="P23" s="11" t="s">
+      <c r="Q23" s="27" t="s">
+        <v>410</v>
+      </c>
+      <c r="R23" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="S23" s="15">
+        <v>100</v>
+      </c>
+      <c r="T23" s="10">
+        <v>100</v>
+      </c>
+      <c r="U23" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="Q23" s="27" t="s">
-        <v>411</v>
-      </c>
-      <c r="R23" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="S23" s="15">
-        <v>100</v>
-      </c>
-      <c r="T23" s="10">
-        <v>100</v>
-      </c>
-      <c r="U23" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>0</v>
       </c>
@@ -5108,17 +5103,17 @@
         <v>6</v>
       </c>
       <c r="O24" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="P24" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="P24" s="12" t="s">
+      <c r="Q24" s="27" t="s">
+        <v>412</v>
+      </c>
+      <c r="R24" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="Q24" s="27" t="s">
-        <v>413</v>
-      </c>
-      <c r="R24" s="11" t="s">
-        <v>68</v>
-      </c>
       <c r="S24" s="13">
         <v>100</v>
       </c>
@@ -5126,12 +5121,12 @@
         <v>100</v>
       </c>
       <c r="U24" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" ht="34" x14ac:dyDescent="0.15">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C25" s="21">
         <v>3</v>
@@ -5140,14 +5135,14 @@
         <v>40</v>
       </c>
       <c r="P25" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q25" s="27" t="s">
+        <v>413</v>
+      </c>
+      <c r="R25" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="Q25" s="27" t="s">
-        <v>414</v>
-      </c>
-      <c r="R25" s="11" t="s">
-        <v>70</v>
-      </c>
       <c r="S25" s="13">
         <v>100</v>
       </c>
@@ -5155,68 +5150,68 @@
         <v>100</v>
       </c>
       <c r="U25" s="10" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" ht="34" x14ac:dyDescent="0.15">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I26" s="21">
         <v>11</v>
       </c>
       <c r="O26" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="P26" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="P26" s="12" t="s">
+      <c r="Q26" s="27" t="s">
+        <v>414</v>
+      </c>
+      <c r="R26" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="Q26" s="27" t="s">
-        <v>415</v>
-      </c>
-      <c r="R26" s="11" t="s">
-        <v>73</v>
-      </c>
       <c r="S26" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="T26" s="14">
         <v>100</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E27" s="21">
         <v>1</v>
       </c>
       <c r="O27" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="P27" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="P27" s="12" t="s">
+      <c r="Q27" s="27" t="s">
+        <v>415</v>
+      </c>
+      <c r="R27" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="Q27" s="27" t="s">
-        <v>416</v>
-      </c>
-      <c r="R27" s="11" t="s">
-        <v>76</v>
-      </c>
       <c r="S27" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="T27" s="14">
         <v>99</v>
       </c>
       <c r="U27" s="10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
@@ -5230,16 +5225,16 @@
         <v>3</v>
       </c>
       <c r="O28" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q28" s="27" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="R28" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S28" s="13">
         <v>100</v>
@@ -5248,12 +5243,12 @@
         <v>100</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B29" s="21">
         <v>3</v>
@@ -5268,30 +5263,30 @@
         <v>6</v>
       </c>
       <c r="O29" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="P29" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="P29" s="12" t="s">
+      <c r="Q29" s="27" t="s">
+        <v>417</v>
+      </c>
+      <c r="R29" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="Q29" s="27" t="s">
-        <v>418</v>
-      </c>
-      <c r="R29" s="11" t="s">
-        <v>79</v>
-      </c>
       <c r="S29" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="T29" s="14">
         <v>100</v>
       </c>
       <c r="U29" s="10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B30" s="21">
         <v>4</v>
@@ -5312,16 +5307,16 @@
         <v>3</v>
       </c>
       <c r="O30" s="11" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="P30" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q30" s="27" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="R30" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S30" s="13">
         <v>100</v>
@@ -5330,97 +5325,97 @@
         <v>92</v>
       </c>
       <c r="U30" s="10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C31" s="21">
         <v>1</v>
       </c>
       <c r="O31" s="11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="P31" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q31" s="27" t="s">
+        <v>419</v>
+      </c>
+      <c r="R31" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="Q31" s="27" t="s">
-        <v>420</v>
-      </c>
-      <c r="R31" s="11" t="s">
-        <v>81</v>
-      </c>
       <c r="S31" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="T31" s="14">
         <v>92</v>
       </c>
       <c r="U31" s="10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F32" s="23">
         <v>1</v>
       </c>
       <c r="O32" s="11" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="P32" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q32" s="27" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="R32" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S32" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="T32" s="14">
         <v>92</v>
       </c>
       <c r="U32" s="10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K33" s="21">
         <v>1</v>
       </c>
       <c r="O33" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="P33" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="P33" s="12" t="s">
-        <v>86</v>
-      </c>
       <c r="Q33" s="27" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="R33" s="11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="S33" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="T33" s="14">
         <v>100</v>
       </c>
       <c r="U33" s="10" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
@@ -5431,17 +5426,17 @@
         <v>1</v>
       </c>
       <c r="O34" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="P34" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="P34" s="12" t="s">
+      <c r="Q34" s="27" t="s">
+        <v>422</v>
+      </c>
+      <c r="R34" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="Q34" s="27" t="s">
-        <v>423</v>
-      </c>
-      <c r="R34" s="11" t="s">
-        <v>89</v>
-      </c>
       <c r="S34" s="13">
         <v>100</v>
       </c>
@@ -5449,10 +5444,10 @@
         <v>100</v>
       </c>
       <c r="U34" s="10" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.15">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>24</v>
       </c>
@@ -5460,12 +5455,12 @@
         <v>1</v>
       </c>
       <c r="Q35" s="28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D36" s="21">
         <v>3</v>
@@ -5486,30 +5481,30 @@
         <v>2</v>
       </c>
       <c r="O36" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="P36" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="P36" s="12" t="s">
+      <c r="Q36" s="27" t="s">
+        <v>423</v>
+      </c>
+      <c r="R36" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="Q36" s="27" t="s">
-        <v>424</v>
-      </c>
-      <c r="R36" s="11" t="s">
-        <v>93</v>
-      </c>
       <c r="S36" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="T36" s="14">
         <v>100</v>
       </c>
       <c r="U36" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E37" s="21">
         <v>11</v>
@@ -5518,16 +5513,16 @@
         <v>11</v>
       </c>
       <c r="O37" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="P37" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="P37" s="12" t="s">
+      <c r="Q37" s="27" t="s">
+        <v>424</v>
+      </c>
+      <c r="R37" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="Q37" s="27" t="s">
-        <v>425</v>
-      </c>
-      <c r="R37" s="11" t="s">
-        <v>96</v>
       </c>
       <c r="S37" s="13">
         <v>99.35</v>
@@ -5536,70 +5531,70 @@
         <v>99</v>
       </c>
       <c r="U37" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F38" s="23">
         <v>9</v>
       </c>
       <c r="O38" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P38" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q38" s="27" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="R38" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S38" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="T38" s="14">
         <v>99</v>
       </c>
       <c r="U38" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B39" s="21">
         <v>5</v>
       </c>
       <c r="O39" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="P39" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="P39" s="12" t="s">
+      <c r="Q39" s="27" t="s">
+        <v>426</v>
+      </c>
+      <c r="R39" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="Q39" s="27" t="s">
-        <v>427</v>
-      </c>
-      <c r="R39" s="11" t="s">
-        <v>100</v>
-      </c>
       <c r="S39" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="T39" s="14">
         <v>100</v>
       </c>
       <c r="U39" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B40" s="21">
         <v>2</v>
@@ -5608,30 +5603,30 @@
         <v>5</v>
       </c>
       <c r="O40" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P40" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q40" s="27" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="R40" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S40" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="T40" s="14">
         <v>100</v>
       </c>
       <c r="U40" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K41" s="21">
         <v>1</v>
@@ -5640,59 +5635,59 @@
         <v>1</v>
       </c>
       <c r="O41" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P41" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q41" s="27" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="R41" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S41" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="T41" s="14">
         <v>100</v>
       </c>
       <c r="U41" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M42" s="21">
         <v>2</v>
       </c>
       <c r="O42" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P42" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q42" s="28" t="s">
+        <v>428</v>
+      </c>
+      <c r="R42" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="Q42" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="R42" s="11" t="s">
-        <v>104</v>
-      </c>
       <c r="S42" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="T42" s="14">
         <v>100</v>
       </c>
       <c r="U42" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" ht="34" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B43" s="21">
         <v>3</v>
@@ -5704,28 +5699,28 @@
         <v>3</v>
       </c>
       <c r="O43" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="P43" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q43" s="27" t="s">
+        <v>429</v>
+      </c>
+      <c r="R43" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="Q43" s="27" t="s">
-        <v>430</v>
-      </c>
-      <c r="R43" s="15" t="s">
-        <v>106</v>
-      </c>
       <c r="S43" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="T43" s="14">
         <v>100</v>
       </c>
       <c r="U43" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>11</v>
       </c>
@@ -5736,16 +5731,16 @@
         <v>2</v>
       </c>
       <c r="O44" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P44" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q44" s="27" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="R44" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S44" s="13">
         <v>100</v>
@@ -5754,10 +5749,10 @@
         <v>100</v>
       </c>
       <c r="U44" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>13</v>
       </c>
@@ -5765,16 +5760,16 @@
         <v>3</v>
       </c>
       <c r="O45" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="P45" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="P45" s="12" t="s">
+      <c r="Q45" s="27" t="s">
+        <v>431</v>
+      </c>
+      <c r="R45" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="Q45" s="27" t="s">
-        <v>432</v>
-      </c>
-      <c r="R45" s="11" t="s">
-        <v>110</v>
       </c>
       <c r="S45" s="13">
         <v>100</v>
@@ -5783,12 +5778,12 @@
         <v>96</v>
       </c>
       <c r="U45" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D46" s="21">
         <v>5</v>
@@ -5800,17 +5795,17 @@
         <v>3</v>
       </c>
       <c r="O46" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="P46" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="P46" s="12" t="s">
+      <c r="Q46" s="28" t="s">
+        <v>432</v>
+      </c>
+      <c r="R46" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="Q46" s="28" t="s">
-        <v>433</v>
-      </c>
-      <c r="R46" s="11" t="s">
-        <v>113</v>
-      </c>
       <c r="S46" s="13">
         <v>100</v>
       </c>
@@ -5818,12 +5813,12 @@
         <v>100</v>
       </c>
       <c r="U46" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" ht="34" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B47" s="21">
         <v>4</v>
@@ -5844,16 +5839,16 @@
         <v>3</v>
       </c>
       <c r="O47" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P47" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="Q47" s="27" t="s">
         <v>436</v>
       </c>
-      <c r="Q47" s="27" t="s">
-        <v>437</v>
-      </c>
       <c r="R47" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S47" s="13">
         <v>100</v>
@@ -5862,12 +5857,12 @@
         <v>100</v>
       </c>
       <c r="U47" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D48" s="21">
         <v>2</v>
@@ -5882,16 +5877,16 @@
         <v>1</v>
       </c>
       <c r="O48" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P48" s="12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="Q48" s="27" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="R48" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S48" s="13">
         <v>100</v>
@@ -5900,41 +5895,41 @@
         <v>100</v>
       </c>
       <c r="U48" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D49" s="21">
         <v>1</v>
       </c>
       <c r="O49" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P49" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q49" s="27" t="s">
+        <v>433</v>
+      </c>
+      <c r="R49" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="Q49" s="27" t="s">
-        <v>434</v>
-      </c>
-      <c r="R49" s="11" t="s">
-        <v>117</v>
-      </c>
       <c r="S49" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T49" s="14">
         <v>100</v>
       </c>
       <c r="U49" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D50" s="21">
         <v>4</v>
@@ -5943,16 +5938,16 @@
         <v>2</v>
       </c>
       <c r="O50" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P50" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q50" s="27" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="R50" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S50" s="13">
         <v>100</v>
@@ -5961,10 +5956,10 @@
         <v>100</v>
       </c>
       <c r="U50" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>4</v>
       </c>
@@ -5975,17 +5970,17 @@
         <v>5</v>
       </c>
       <c r="O51" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="P51" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="P51" s="12" t="s">
+      <c r="Q51" s="27" t="s">
+        <v>439</v>
+      </c>
+      <c r="R51" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="Q51" s="27" t="s">
-        <v>440</v>
-      </c>
-      <c r="R51" s="11" t="s">
-        <v>121</v>
-      </c>
       <c r="S51" s="13">
         <v>100</v>
       </c>
@@ -5993,28 +5988,28 @@
         <v>100</v>
       </c>
       <c r="U51" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G52" s="21">
         <v>3</v>
       </c>
       <c r="O52" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P52" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q52" s="27" t="s">
+        <v>440</v>
+      </c>
+      <c r="R52" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="Q52" s="27" t="s">
-        <v>441</v>
-      </c>
-      <c r="R52" s="11" t="s">
-        <v>123</v>
-      </c>
       <c r="S52" s="13">
         <v>100</v>
       </c>
@@ -6022,28 +6017,28 @@
         <v>100</v>
       </c>
       <c r="U52" s="10" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G53" s="21">
         <v>4</v>
       </c>
       <c r="O53" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P53" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q53" s="27" t="s">
+        <v>441</v>
+      </c>
+      <c r="R53" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="Q53" s="27" t="s">
-        <v>442</v>
-      </c>
-      <c r="R53" s="11" t="s">
-        <v>125</v>
-      </c>
       <c r="S53" s="13">
         <v>100</v>
       </c>
@@ -6051,10 +6046,10 @@
         <v>100</v>
       </c>
       <c r="U53" s="10" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>2</v>
       </c>
@@ -6065,16 +6060,16 @@
         <v>2</v>
       </c>
       <c r="O54" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="P54" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="P54" s="12" t="s">
+      <c r="Q54" s="27" t="s">
+        <v>442</v>
+      </c>
+      <c r="R54" s="11" t="s">
         <v>127</v>
-      </c>
-      <c r="Q54" s="27" t="s">
-        <v>443</v>
-      </c>
-      <c r="R54" s="11" t="s">
-        <v>128</v>
       </c>
       <c r="S54" s="13">
         <v>100</v>
@@ -6083,10 +6078,10 @@
         <v>98</v>
       </c>
       <c r="U54" s="10" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>17</v>
       </c>
@@ -6097,16 +6092,16 @@
         <v>1</v>
       </c>
       <c r="O55" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="P55" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="P55" s="12" t="s">
+      <c r="Q55" s="27" t="s">
+        <v>443</v>
+      </c>
+      <c r="R55" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="Q55" s="27" t="s">
-        <v>444</v>
-      </c>
-      <c r="R55" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="S55" s="13">
         <v>100</v>
@@ -6115,10 +6110,10 @@
         <v>98</v>
       </c>
       <c r="U55" s="10" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" ht="34" x14ac:dyDescent="0.15">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>10</v>
       </c>
@@ -6129,17 +6124,17 @@
         <v>2</v>
       </c>
       <c r="O56" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="P56" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="P56" s="12" t="s">
+      <c r="Q56" s="27" t="s">
+        <v>450</v>
+      </c>
+      <c r="R56" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="Q56" s="27" t="s">
-        <v>451</v>
-      </c>
-      <c r="R56" s="11" t="s">
-        <v>134</v>
-      </c>
       <c r="S56" s="13">
         <v>100</v>
       </c>
@@ -6147,12 +6142,12 @@
         <v>100</v>
       </c>
       <c r="U56" s="10" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C57" s="21">
         <v>5</v>
@@ -6161,75 +6156,75 @@
         <v>1</v>
       </c>
       <c r="O57" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="P57" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="P57" s="12" t="s">
+      <c r="Q57" s="27" t="s">
+        <v>444</v>
+      </c>
+      <c r="R57" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="Q57" s="27" t="s">
-        <v>445</v>
-      </c>
-      <c r="R57" s="11" t="s">
-        <v>137</v>
-      </c>
       <c r="S57" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T57" s="14">
         <v>100</v>
       </c>
       <c r="U57" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H58" s="21">
         <v>2</v>
       </c>
       <c r="O58" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="P58" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="P58" s="12" t="s">
+      <c r="Q58" s="27" t="s">
+        <v>445</v>
+      </c>
+      <c r="R58" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="Q58" s="27" t="s">
-        <v>446</v>
-      </c>
-      <c r="R58" s="11" t="s">
-        <v>140</v>
-      </c>
       <c r="S58" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="T58" s="14">
         <v>100</v>
       </c>
       <c r="U58" s="10" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H59" s="21">
         <v>3</v>
       </c>
       <c r="O59" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="P59" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q59" s="27" t="s">
+        <v>446</v>
+      </c>
+      <c r="R59" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="Q59" s="27" t="s">
-        <v>447</v>
-      </c>
-      <c r="R59" s="11" t="s">
-        <v>143</v>
-      </c>
       <c r="S59" s="13">
         <v>100</v>
       </c>
@@ -6237,41 +6232,41 @@
         <v>100</v>
       </c>
       <c r="U59" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D60" s="21">
         <v>1</v>
       </c>
       <c r="O60" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="P60" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q60" s="27" t="s">
+        <v>447</v>
+      </c>
+      <c r="R60" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="Q60" s="27" t="s">
-        <v>448</v>
-      </c>
-      <c r="R60" s="11" t="s">
-        <v>145</v>
-      </c>
       <c r="S60" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="T60" s="14">
         <v>99</v>
       </c>
       <c r="U60" s="10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21" ht="34" x14ac:dyDescent="0.15">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F61" s="23">
         <v>1</v>
@@ -6280,146 +6275,146 @@
         <v>2</v>
       </c>
       <c r="O61" s="11" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="P61" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q61" s="27" t="s">
+        <v>448</v>
+      </c>
+      <c r="R61" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="Q61" s="27" t="s">
-        <v>449</v>
-      </c>
-      <c r="R61" s="11" t="s">
-        <v>147</v>
-      </c>
       <c r="S61" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="T61" s="14">
         <v>100</v>
       </c>
       <c r="U61" s="10" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B62" s="24">
         <v>6</v>
       </c>
       <c r="O62" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P62" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q62" s="27" t="s">
+        <v>390</v>
+      </c>
+      <c r="R62" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="Q62" s="27" t="s">
-        <v>391</v>
-      </c>
-      <c r="R62" s="15" t="s">
+      <c r="S62" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="T62" s="14">
+        <v>100</v>
+      </c>
+      <c r="U62" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="S62" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="T62" s="14">
-        <v>100</v>
-      </c>
-      <c r="U62" s="15" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="63" spans="1:21" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N63" s="24">
         <v>1</v>
       </c>
       <c r="O63" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="P63" s="13" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Q63" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="R63" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="S63" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="S63" s="13" t="s">
-        <v>334</v>
-      </c>
       <c r="T63" s="13">
         <v>100</v>
       </c>
       <c r="U63" s="15" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B64" s="24">
         <v>1</v>
       </c>
       <c r="O64" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P64" s="13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Q64" s="28" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="R64" s="15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="S64" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="T64" s="13">
         <v>100</v>
       </c>
       <c r="U64" s="15" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="65" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K65" s="21">
         <v>2</v>
       </c>
       <c r="O65" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P65" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Q65" s="27" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="R65" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="S65" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="T65" s="14">
         <v>100</v>
       </c>
       <c r="U65" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="66" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E66" s="21">
         <v>1</v>
@@ -6434,16 +6429,16 @@
         <v>1</v>
       </c>
       <c r="O66" s="11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P66" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q66" s="28" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="R66" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S66" s="13">
         <v>100</v>
@@ -6452,86 +6447,86 @@
         <v>100</v>
       </c>
       <c r="U66" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J67" s="21">
         <v>1</v>
       </c>
       <c r="O67" s="11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P67" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q67" s="27" t="s">
+        <v>451</v>
+      </c>
+      <c r="R67" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="Q67" s="27" t="s">
-        <v>452</v>
-      </c>
-      <c r="R67" s="11" t="s">
-        <v>150</v>
-      </c>
       <c r="S67" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="T67" s="14">
         <v>100</v>
       </c>
       <c r="U67" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C68" s="21">
         <v>1</v>
       </c>
       <c r="O68" s="11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P68" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q68" s="27" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="R68" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S68" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="T68" s="14">
         <v>100</v>
       </c>
       <c r="U68" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21" ht="34" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B69" s="21">
         <v>1</v>
       </c>
       <c r="O69" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P69" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q69" s="28" t="s">
+        <v>459</v>
+      </c>
+      <c r="R69" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="Q69" s="28" t="s">
-        <v>460</v>
-      </c>
-      <c r="R69" s="11" t="s">
-        <v>154</v>
-      </c>
       <c r="S69" s="13">
         <v>100</v>
       </c>
@@ -6539,12 +6534,12 @@
         <v>100</v>
       </c>
       <c r="U69" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="70" spans="1:21" ht="34" customHeight="1" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D70" s="21">
         <v>7</v>
@@ -6553,17 +6548,17 @@
         <v>1</v>
       </c>
       <c r="O70" s="11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="P70" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q70" s="27" t="s">
+        <v>453</v>
+      </c>
+      <c r="R70" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="Q70" s="27" t="s">
-        <v>454</v>
-      </c>
-      <c r="R70" s="11" t="s">
-        <v>156</v>
-      </c>
       <c r="S70" s="13">
         <v>100</v>
       </c>
@@ -6571,28 +6566,28 @@
         <v>100</v>
       </c>
       <c r="U70" s="10" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="71" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F71" s="23">
         <v>4</v>
       </c>
       <c r="O71" s="11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="P71" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q71" s="27" t="s">
+        <v>454</v>
+      </c>
+      <c r="R71" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="Q71" s="27" t="s">
-        <v>455</v>
-      </c>
-      <c r="R71" s="11" t="s">
-        <v>158</v>
-      </c>
       <c r="S71" s="13">
         <v>100</v>
       </c>
@@ -6600,39 +6595,39 @@
         <v>100</v>
       </c>
       <c r="U71" s="10" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="72" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F72" s="23">
         <v>4</v>
       </c>
       <c r="O72" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="P72" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="P72" s="12" t="s">
+      <c r="Q72" s="27" t="s">
+        <v>455</v>
+      </c>
+      <c r="R72" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="Q72" s="27" t="s">
-        <v>456</v>
-      </c>
-      <c r="R72" s="11" t="s">
-        <v>161</v>
-      </c>
       <c r="S72" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="T72" s="14">
         <v>100</v>
       </c>
       <c r="U72" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>14</v>
       </c>
@@ -6640,16 +6635,16 @@
         <v>1</v>
       </c>
       <c r="O73" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="P73" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="P73" s="12" t="s">
+      <c r="Q73" s="27" t="s">
+        <v>456</v>
+      </c>
+      <c r="R73" s="11" t="s">
         <v>163</v>
-      </c>
-      <c r="Q73" s="27" t="s">
-        <v>457</v>
-      </c>
-      <c r="R73" s="11" t="s">
-        <v>164</v>
       </c>
       <c r="S73" s="13">
         <v>100</v>
@@ -6658,10 +6653,10 @@
         <v>99</v>
       </c>
       <c r="U73" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>19</v>
       </c>
@@ -6669,16 +6664,16 @@
         <v>4</v>
       </c>
       <c r="O74" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="P74" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="P74" s="12" t="s">
+      <c r="Q74" s="27" t="s">
+        <v>457</v>
+      </c>
+      <c r="R74" s="11" t="s">
         <v>166</v>
-      </c>
-      <c r="Q74" s="27" t="s">
-        <v>458</v>
-      </c>
-      <c r="R74" s="11" t="s">
-        <v>167</v>
       </c>
       <c r="S74" s="13">
         <v>100</v>
@@ -6687,41 +6682,41 @@
         <v>92</v>
       </c>
       <c r="U74" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="75" spans="1:21" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D75" s="21">
         <v>1</v>
       </c>
       <c r="O75" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="P75" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="P75" s="12" t="s">
+      <c r="Q75" s="27" t="s">
+        <v>458</v>
+      </c>
+      <c r="R75" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="Q75" s="27" t="s">
-        <v>459</v>
-      </c>
-      <c r="R75" s="11" t="s">
-        <v>170</v>
-      </c>
       <c r="S75" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="T75" s="14">
         <v>100</v>
       </c>
       <c r="U75" s="10" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="76" spans="1:21" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" ht="19.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G76" s="21">
         <v>4</v>
@@ -6730,17 +6725,17 @@
         <v>4</v>
       </c>
       <c r="O76" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="P76" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="P76" s="12" t="s">
+      <c r="Q76" s="28" t="s">
+        <v>469</v>
+      </c>
+      <c r="R76" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="Q76" s="28" t="s">
-        <v>470</v>
-      </c>
-      <c r="R76" s="11" t="s">
-        <v>173</v>
-      </c>
       <c r="S76" s="13">
         <v>100</v>
       </c>
@@ -6748,27 +6743,27 @@
         <v>100</v>
       </c>
       <c r="U76" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="77" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E77" s="21">
         <v>2</v>
       </c>
       <c r="O77" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="P77" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="P77" s="12" t="s">
+      <c r="Q77" s="27" t="s">
+        <v>461</v>
+      </c>
+      <c r="R77" s="11" t="s">
         <v>183</v>
-      </c>
-      <c r="Q77" s="27" t="s">
-        <v>462</v>
-      </c>
-      <c r="R77" s="11" t="s">
-        <v>184</v>
       </c>
       <c r="S77" s="13">
         <v>100</v>
@@ -6777,41 +6772,41 @@
         <v>99</v>
       </c>
       <c r="U77" s="10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="78" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F78" s="23">
         <v>2</v>
       </c>
       <c r="O78" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="P78" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="P78" s="12" t="s">
+      <c r="Q78" s="27" t="s">
+        <v>462</v>
+      </c>
+      <c r="R78" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="Q78" s="27" t="s">
-        <v>463</v>
-      </c>
-      <c r="R78" s="11" t="s">
-        <v>176</v>
-      </c>
       <c r="S78" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="T78" s="14">
         <v>100</v>
       </c>
       <c r="U78" s="10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="79" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B79" s="21">
         <v>4</v>
@@ -6829,59 +6824,59 @@
         <v>3</v>
       </c>
       <c r="O79" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="P79" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="P79" s="12" t="s">
-        <v>178</v>
-      </c>
       <c r="Q79" s="27" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="R79" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S79" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="T79" s="14">
         <v>100</v>
       </c>
       <c r="U79" s="10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="80" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B80" s="21">
         <v>5</v>
       </c>
       <c r="O80" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P80" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q80" s="27" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="R80" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S80" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="T80" s="14">
         <v>100</v>
       </c>
       <c r="U80" s="10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="81" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B81" s="21">
         <v>6</v>
@@ -6896,57 +6891,57 @@
         <v>4</v>
       </c>
       <c r="O81" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P81" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q81" s="27" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="R81" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S81" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="T81" s="14">
         <v>100</v>
       </c>
       <c r="U81" s="10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="82" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C82" s="21">
         <v>5</v>
       </c>
       <c r="O82" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P82" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Q82" s="27" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="R82" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S82" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="T82" s="14">
         <v>100</v>
       </c>
       <c r="U82" s="10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="83" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>1</v>
       </c>
@@ -6960,17 +6955,17 @@
         <v>1</v>
       </c>
       <c r="O83" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="P83" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="P83" s="12" t="s">
+      <c r="Q83" s="27" t="s">
+        <v>467</v>
+      </c>
+      <c r="R83" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="Q83" s="27" t="s">
-        <v>468</v>
-      </c>
-      <c r="R83" s="11" t="s">
-        <v>187</v>
-      </c>
       <c r="S83" s="13">
         <v>100</v>
       </c>
@@ -6978,12 +6973,12 @@
         <v>100</v>
       </c>
       <c r="U83" s="10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="84" spans="1:21" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E84" s="21">
         <v>6</v>
@@ -6992,30 +6987,30 @@
         <v>1</v>
       </c>
       <c r="O84" s="11" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="P84" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q84" s="27" t="s">
+        <v>468</v>
+      </c>
+      <c r="R84" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="Q84" s="27" t="s">
-        <v>469</v>
-      </c>
-      <c r="R84" s="11" t="s">
-        <v>189</v>
-      </c>
       <c r="S84" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T84" s="14">
         <v>100</v>
       </c>
       <c r="U84" s="10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="85" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C85" s="24">
         <v>1</v>
@@ -7024,54 +7019,54 @@
         <v>1</v>
       </c>
       <c r="O85" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P85" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q85" s="27" t="s">
+        <v>393</v>
+      </c>
+      <c r="R85" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="Q85" s="27" t="s">
-        <v>394</v>
-      </c>
-      <c r="R85" s="15" t="s">
+      <c r="S85" s="13" t="s">
         <v>321</v>
       </c>
-      <c r="S85" s="13" t="s">
-        <v>322</v>
-      </c>
       <c r="T85" s="13">
         <v>100</v>
       </c>
       <c r="U85" s="15" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="86" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I86" s="24">
         <v>1</v>
       </c>
       <c r="O86" s="15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P86" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q86" s="27" t="s">
+        <v>394</v>
+      </c>
+      <c r="S86" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="T86" s="13">
+        <v>100</v>
+      </c>
+      <c r="U86" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="Q86" s="27" t="s">
-        <v>395</v>
-      </c>
-      <c r="S86" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="T86" s="13">
-        <v>100</v>
-      </c>
-      <c r="U86" s="15" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="87" spans="1:21" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="87" spans="1:21" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>18</v>
       </c>
@@ -7079,17 +7074,17 @@
         <v>1</v>
       </c>
       <c r="O87" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="P87" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="P87" s="12" t="s">
+      <c r="Q87" s="27" t="s">
+        <v>470</v>
+      </c>
+      <c r="R87" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="Q87" s="27" t="s">
-        <v>471</v>
-      </c>
-      <c r="R87" s="11" t="s">
-        <v>192</v>
-      </c>
       <c r="S87" s="13">
         <v>100</v>
       </c>
@@ -7097,39 +7092,39 @@
         <v>100</v>
       </c>
       <c r="U87" s="10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="88" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D88" s="21">
         <v>2</v>
       </c>
       <c r="O88" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="P88" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="P88" s="12" t="s">
+      <c r="Q88" s="27" t="s">
+        <v>471</v>
+      </c>
+      <c r="R88" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="Q88" s="27" t="s">
-        <v>472</v>
-      </c>
-      <c r="R88" s="11" t="s">
-        <v>195</v>
-      </c>
       <c r="S88" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="T88" s="14">
         <v>100</v>
       </c>
       <c r="U88" s="10" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="89" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>16</v>
       </c>
@@ -7140,17 +7135,17 @@
         <v>3</v>
       </c>
       <c r="O89" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="P89" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="P89" s="12" t="s">
+      <c r="Q89" s="27" t="s">
+        <v>472</v>
+      </c>
+      <c r="R89" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="Q89" s="27" t="s">
-        <v>473</v>
-      </c>
-      <c r="R89" s="11" t="s">
-        <v>198</v>
-      </c>
       <c r="S89" s="13">
         <v>100</v>
       </c>
@@ -7158,10 +7153,10 @@
         <v>100</v>
       </c>
       <c r="U89" s="10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="90" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>21</v>
       </c>
@@ -7169,17 +7164,17 @@
         <v>1</v>
       </c>
       <c r="O90" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="P90" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="P90" s="12" t="s">
+      <c r="Q90" s="27" t="s">
+        <v>473</v>
+      </c>
+      <c r="R90" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="Q90" s="27" t="s">
-        <v>474</v>
-      </c>
-      <c r="R90" s="11" t="s">
-        <v>201</v>
-      </c>
       <c r="S90" s="13">
         <v>100</v>
       </c>
@@ -7187,10 +7182,10 @@
         <v>100</v>
       </c>
       <c r="U90" s="10" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="91" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>7</v>
       </c>
@@ -7198,17 +7193,17 @@
         <v>1</v>
       </c>
       <c r="O91" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="P91" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="P91" s="12" t="s">
+      <c r="Q91" s="27" t="s">
+        <v>474</v>
+      </c>
+      <c r="R91" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="Q91" s="27" t="s">
-        <v>475</v>
-      </c>
-      <c r="R91" s="11" t="s">
-        <v>204</v>
-      </c>
       <c r="S91" s="13">
         <v>100</v>
       </c>
@@ -7216,10 +7211,10 @@
         <v>100</v>
       </c>
       <c r="U91" s="10" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="92" spans="1:21" ht="17" x14ac:dyDescent="0.15">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>22</v>
       </c>
@@ -7230,17 +7225,17 @@
         <v>3</v>
       </c>
       <c r="O92" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="P92" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="P92" s="12" t="s">
+      <c r="Q92" s="27" t="s">
+        <v>475</v>
+      </c>
+      <c r="R92" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="Q92" s="27" t="s">
-        <v>476</v>
-      </c>
-      <c r="R92" s="11" t="s">
-        <v>207</v>
-      </c>
       <c r="S92" s="13">
         <v>100</v>
       </c>
@@ -7248,12 +7243,12 @@
         <v>100</v>
       </c>
       <c r="U92" s="10" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.15">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B93" s="20">
         <f>SUM(B3:B91)</f>

</xml_diff>